<commit_message>
Update CT and test data
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/amendment_1.xlsx
+++ b/tests/integration_test_files/amendment_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E60300-1767-1442-B3EF-8CC39F105C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CE7814-C2A1-7C48-8893-4187A635899E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="59880" yWindow="4900" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="592">
   <si>
     <t>Epoch</t>
   </si>
@@ -1850,6 +1850,12 @@
   </si>
   <si>
     <t>enrollment</t>
+  </si>
+  <si>
+    <t>Fix typos</t>
+  </si>
+  <si>
+    <t>Other=Fix typographical errors</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +1939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2017,6 +2023,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4831,94 +4843,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051C019D-8DBE-D14B-A9B5-0060B58D7557}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" style="7" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="6" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
         <v>573</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>574</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>575</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>576</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>577</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="33" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>4</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>579</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="11" t="s">
         <v>581</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>578</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>582</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>583</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>584</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>586</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>590</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>580</v>
       </c>
-      <c r="D4" t="s">
-        <v>584</v>
-      </c>
-      <c r="E4" t="s">
-        <v>585</v>
-      </c>
-      <c r="F4" t="s">
-        <v>586</v>
-      </c>
+      <c r="D5" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweak excel test file
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/amendment_1.xlsx
+++ b/tests/integration_test_files/amendment_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C2C85-D673-2741-B471-DABCDFD044CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9818FB2-4FB4-0C4C-98D6-2EEC94AB311A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59880" yWindow="4900" windowWidth="33600" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="59880" yWindow="4900" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -2349,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4846,10 +4846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051C019D-8DBE-D14B-A9B5-0060B58D7557}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4960,15 +4960,6 @@
         <v>590</v>
       </c>
       <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add in document reference for amendment changes
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/amendment_1.xlsx
+++ b/tests/integration_test_files/amendment_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC11BB27-27D5-F243-883F-2D9C4733FA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD347573-AC53-554C-ABBC-B12CFE0D6C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53380" yWindow="4760" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="20100" yWindow="500" windowWidth="53160" windowHeight="27240" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -32,8 +32,9 @@
     <sheet name="studyDesignProcedures" sheetId="11" r:id="rId17"/>
     <sheet name="studyDesignEncounters" sheetId="12" r:id="rId18"/>
     <sheet name="studyDesignElements" sheetId="13" r:id="rId19"/>
-    <sheet name="studyDesignContent" sheetId="17" r:id="rId20"/>
-    <sheet name="configuration" sheetId="10" r:id="rId21"/>
+    <sheet name="document" sheetId="23" r:id="rId20"/>
+    <sheet name="documentContent" sheetId="17" r:id="rId21"/>
+    <sheet name="configuration" sheetId="10" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="849">
   <si>
     <t>Screening</t>
   </si>
@@ -2205,6 +2206,432 @@
   </si>
   <si>
     <t>AMEND_DATE_4</t>
+  </si>
+  <si>
+    <t>displaySectionNumber</t>
+  </si>
+  <si>
+    <t>displaySectionTitle</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>NC_1</t>
+  </si>
+  <si>
+    <t>NC_2</t>
+  </si>
+  <si>
+    <t>NC_3</t>
+  </si>
+  <si>
+    <t>NC_4</t>
+  </si>
+  <si>
+    <t>NC_5</t>
+  </si>
+  <si>
+    <t>NC_6</t>
+  </si>
+  <si>
+    <t>NC_7</t>
+  </si>
+  <si>
+    <t>NC_8</t>
+  </si>
+  <si>
+    <t>NC_9</t>
+  </si>
+  <si>
+    <t>NC_10</t>
+  </si>
+  <si>
+    <t>NC_11</t>
+  </si>
+  <si>
+    <t>NC_12</t>
+  </si>
+  <si>
+    <t>NC_13</t>
+  </si>
+  <si>
+    <t>NC_14</t>
+  </si>
+  <si>
+    <t>NC_15</t>
+  </si>
+  <si>
+    <t>NC_16</t>
+  </si>
+  <si>
+    <t>NC_17</t>
+  </si>
+  <si>
+    <t>NC_18</t>
+  </si>
+  <si>
+    <t>NC_19</t>
+  </si>
+  <si>
+    <t>NC_20</t>
+  </si>
+  <si>
+    <t>NC_21</t>
+  </si>
+  <si>
+    <t>NC_22</t>
+  </si>
+  <si>
+    <t>NC_23</t>
+  </si>
+  <si>
+    <t>NC_24</t>
+  </si>
+  <si>
+    <t>NC_25</t>
+  </si>
+  <si>
+    <t>NC_26</t>
+  </si>
+  <si>
+    <t>NC_27</t>
+  </si>
+  <si>
+    <t>NC_28</t>
+  </si>
+  <si>
+    <t>NC_29</t>
+  </si>
+  <si>
+    <t>NC_30</t>
+  </si>
+  <si>
+    <t>NC_31</t>
+  </si>
+  <si>
+    <t>NC_32</t>
+  </si>
+  <si>
+    <t>NC_33</t>
+  </si>
+  <si>
+    <t>NC_34</t>
+  </si>
+  <si>
+    <t>NC_35</t>
+  </si>
+  <si>
+    <t>NC_36</t>
+  </si>
+  <si>
+    <t>NC_37</t>
+  </si>
+  <si>
+    <t>NC_38</t>
+  </si>
+  <si>
+    <t>NC_39</t>
+  </si>
+  <si>
+    <t>NC_40</t>
+  </si>
+  <si>
+    <t>NC_41</t>
+  </si>
+  <si>
+    <t>NC_42</t>
+  </si>
+  <si>
+    <t>NC_43</t>
+  </si>
+  <si>
+    <t>NC_44</t>
+  </si>
+  <si>
+    <t>NC_45</t>
+  </si>
+  <si>
+    <t>NC_46</t>
+  </si>
+  <si>
+    <t>NC_47</t>
+  </si>
+  <si>
+    <t>NC_48</t>
+  </si>
+  <si>
+    <t>NC_49</t>
+  </si>
+  <si>
+    <t>NC_50</t>
+  </si>
+  <si>
+    <t>NC_51</t>
+  </si>
+  <si>
+    <t>NC_52</t>
+  </si>
+  <si>
+    <t>NC_53</t>
+  </si>
+  <si>
+    <t>NC_54</t>
+  </si>
+  <si>
+    <t>NC_55</t>
+  </si>
+  <si>
+    <t>NC_56</t>
+  </si>
+  <si>
+    <t>NC_57</t>
+  </si>
+  <si>
+    <t>NC_58</t>
+  </si>
+  <si>
+    <t>NC_59</t>
+  </si>
+  <si>
+    <t>NC_60</t>
+  </si>
+  <si>
+    <t>NC_61</t>
+  </si>
+  <si>
+    <t>NC_62</t>
+  </si>
+  <si>
+    <t>NC_63</t>
+  </si>
+  <si>
+    <t>NC_64</t>
+  </si>
+  <si>
+    <t>NC_65</t>
+  </si>
+  <si>
+    <t>NC_66</t>
+  </si>
+  <si>
+    <t>NC_67</t>
+  </si>
+  <si>
+    <t>NC_68</t>
+  </si>
+  <si>
+    <t>NC_69</t>
+  </si>
+  <si>
+    <t>NC_70</t>
+  </si>
+  <si>
+    <t>NC_71</t>
+  </si>
+  <si>
+    <t>NC_72</t>
+  </si>
+  <si>
+    <t>NC_73</t>
+  </si>
+  <si>
+    <t>NC_74</t>
+  </si>
+  <si>
+    <t>NC_75</t>
+  </si>
+  <si>
+    <t>NC_76</t>
+  </si>
+  <si>
+    <t>NC_77</t>
+  </si>
+  <si>
+    <t>NC_78</t>
+  </si>
+  <si>
+    <t>NC_79</t>
+  </si>
+  <si>
+    <t>NC_80</t>
+  </si>
+  <si>
+    <t>NC_81</t>
+  </si>
+  <si>
+    <t>NC_82</t>
+  </si>
+  <si>
+    <t>NC_83</t>
+  </si>
+  <si>
+    <t>NC_84</t>
+  </si>
+  <si>
+    <t>NC_85</t>
+  </si>
+  <si>
+    <t>NC_86</t>
+  </si>
+  <si>
+    <t>NC_87</t>
+  </si>
+  <si>
+    <t>NC_88</t>
+  </si>
+  <si>
+    <t>NC_89</t>
+  </si>
+  <si>
+    <t>NC_90</t>
+  </si>
+  <si>
+    <t>NC_91</t>
+  </si>
+  <si>
+    <t>NC_92</t>
+  </si>
+  <si>
+    <t>NC_93</t>
+  </si>
+  <si>
+    <t>NC_94</t>
+  </si>
+  <si>
+    <t>NC_95</t>
+  </si>
+  <si>
+    <t>NC_96</t>
+  </si>
+  <si>
+    <t>NC_97</t>
+  </si>
+  <si>
+    <t>NC_98</t>
+  </si>
+  <si>
+    <t>NC_99</t>
+  </si>
+  <si>
+    <t>NC_100</t>
+  </si>
+  <si>
+    <t>NC_101</t>
+  </si>
+  <si>
+    <t>NC_102</t>
+  </si>
+  <si>
+    <t>NC_103</t>
+  </si>
+  <si>
+    <t>NC_104</t>
+  </si>
+  <si>
+    <t>NC_105</t>
+  </si>
+  <si>
+    <t>NC_106</t>
+  </si>
+  <si>
+    <t>NC_107</t>
+  </si>
+  <si>
+    <t>NC_108</t>
+  </si>
+  <si>
+    <t>NC_109</t>
+  </si>
+  <si>
+    <t>NC_110</t>
+  </si>
+  <si>
+    <t>NC_111</t>
+  </si>
+  <si>
+    <t>NC_112</t>
+  </si>
+  <si>
+    <t>NC_113</t>
+  </si>
+  <si>
+    <t>NC_114</t>
+  </si>
+  <si>
+    <t>NC_115</t>
+  </si>
+  <si>
+    <t>NC_116</t>
+  </si>
+  <si>
+    <t>NC_117</t>
+  </si>
+  <si>
+    <t>NC_118</t>
+  </si>
+  <si>
+    <t>NC_119</t>
+  </si>
+  <si>
+    <t>NC_120</t>
+  </si>
+  <si>
+    <t>NC_121</t>
+  </si>
+  <si>
+    <t>NC_122</t>
+  </si>
+  <si>
+    <t>NC_123</t>
+  </si>
+  <si>
+    <t>NC_124</t>
+  </si>
+  <si>
+    <t>NC_125</t>
+  </si>
+  <si>
+    <t>NC_126</t>
+  </si>
+  <si>
+    <t>NC_127</t>
+  </si>
+  <si>
+    <t>NC_128</t>
+  </si>
+  <si>
+    <t>NC_129</t>
+  </si>
+  <si>
+    <t>NC_130</t>
+  </si>
+  <si>
+    <t>NC_131</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>NCI_1</t>
+  </si>
+  <si>
+    <t>NCI_2</t>
+  </si>
+  <si>
+    <t>NCI_3</t>
+  </si>
+  <si>
+    <t>NCI_4</t>
+  </si>
+  <si>
+    <t>NCI_5</t>
+  </si>
+  <si>
+    <t>NCI_BLANK</t>
+  </si>
+  <si>
+    <t>document</t>
   </si>
 </sst>
 </file>
@@ -2294,7 +2721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2373,10 +2800,25 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4677,10 +5119,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051C019D-8DBE-D14B-A9B5-0060B58D7557}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4693,7 +5135,7 @@
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>532</v>
       </c>
@@ -4715,8 +5157,11 @@
       <c r="G1" s="27" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="18" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>388</v>
       </c>
@@ -4736,8 +5181,11 @@
       <c r="G2" s="10" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="10" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>387</v>
       </c>
@@ -4757,8 +5205,11 @@
       <c r="G3" s="10" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="10" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>384</v>
       </c>
@@ -4778,8 +5229,11 @@
       <c r="G4" s="10" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="10" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -4798,6 +5252,9 @@
       </c>
       <c r="G5" s="10" t="s">
         <v>706</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>848</v>
       </c>
     </row>
   </sheetData>
@@ -4806,1246 +5263,2690 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
-  <dimension ref="A1:D138"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DB12B0-8474-5047-A986-AD63A7E57931}">
+  <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45:F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="3" width="49.83203125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="81.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46" style="14" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>446</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>486</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>446</v>
-      </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="33" t="s">
+        <v>707</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
+      <c r="E1" s="33" t="s">
+        <v>708</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>710</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E2" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>711</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E3" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>712</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E4" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>383</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E5" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E6" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>715</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E7" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
+        <v>716</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E8" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>717</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="E9" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>718</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>515</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E10" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
+        <v>719</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E11" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>389</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E12" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E13" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
+        <v>722</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E14" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
+        <v>723</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E15" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
+        <v>724</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E16" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
+        <v>725</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>726</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E18" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
+        <v>727</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E19" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
+        <v>728</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E20" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
+        <v>729</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E21" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
+        <v>730</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="E22" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="E23" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
+        <v>732</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E24" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
+        <v>733</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E25" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
+        <v>734</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E27" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
+        <v>736</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>438</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E28" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
+        <v>737</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E29" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E30" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E31" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
+        <v>740</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D32" s="14" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E32" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
+        <v>741</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E33" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
+        <v>742</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E34" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
+        <v>743</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E35" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
+        <v>744</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>480</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E36" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D37" s="14" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E37" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
+        <v>746</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E38" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
+        <v>747</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D39" s="14" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E39" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
+        <v>748</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E40" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
+        <v>749</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>482</v>
       </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E41" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
+        <v>750</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E42" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
+        <v>751</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E43" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E44" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E45" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
+        <v>754</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E46" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
+        <v>755</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="B47" s="23"/>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E47" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
+        <v>756</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E48" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
+        <v>757</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E49" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D50" s="14" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E50" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
+        <v>759</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D51" s="14" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E51" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
+        <v>760</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="B52" s="23"/>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E52" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
+        <v>761</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D53" s="14" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E53" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D54" s="14" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E54" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D55" s="14" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E55" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E56" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
+        <v>765</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="B57" s="23"/>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E57" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="B58" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="B58" s="23"/>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E58" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E59" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
+        <v>768</v>
+      </c>
+      <c r="B60" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E60" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
+        <v>769</v>
+      </c>
+      <c r="B61" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="B61" s="23"/>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D61" s="14" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E61" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="B62" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D62" s="14" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E62" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="B63" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E63" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="B64" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="B64" s="23"/>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E64" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B65" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="B65" s="23"/>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D65" s="14" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E65" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
+        <v>774</v>
+      </c>
+      <c r="B66" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="B66" s="23"/>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D66" s="14" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E66" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="B67" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="B67" s="23"/>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D67" s="14" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E67" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="B68" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="B68" s="23"/>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D68" s="14" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E68" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="B69" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="B69" s="23"/>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D69" s="14" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E69" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="B70" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="B70" s="23"/>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D70" s="14" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E70" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="B71" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="B71" s="23"/>
-      <c r="C71" s="9" t="s">
+      <c r="C71" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D71" s="14" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E71" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="B72" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="B72" s="23"/>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D72" s="14" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E72" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="B73" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D73" s="14" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E73" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
+        <v>782</v>
+      </c>
+      <c r="B74" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="B74" s="23"/>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D74" s="14" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E74" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="B75" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="B75" s="23"/>
-      <c r="C75" s="9" t="s">
+      <c r="C75" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D75" s="14" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E75" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="B76" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="B76" s="23"/>
-      <c r="C76" s="9" t="s">
+      <c r="C76" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D76" s="14" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E76" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="B77" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="B77" s="23"/>
-      <c r="C77" s="9" t="s">
+      <c r="C77" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D77" s="14" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E77" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="B78" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="B78" s="23"/>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D78" s="14" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E78" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="B79" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D79" s="14" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E79" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
+        <v>788</v>
+      </c>
+      <c r="B80" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="B80" s="23"/>
-      <c r="C80" s="9" t="s">
+      <c r="C80" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D80" s="14" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E80" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
+        <v>789</v>
+      </c>
+      <c r="B81" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="B81" s="23"/>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D81" s="14" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E81" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F81" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="B82" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="B82" s="23"/>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D82" s="14" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E82" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="B83" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="B83" s="23"/>
-      <c r="C83" s="9" t="s">
+      <c r="C83" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D83" s="14" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E83" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="B84" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="B84" s="23"/>
-      <c r="C84" s="9" t="s">
+      <c r="C84" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D84" s="14" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E84" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="B85" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="B85" s="23"/>
-      <c r="C85" s="9" t="s">
+      <c r="C85" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D85" s="14" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E85" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="B86" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="B86" s="23"/>
-      <c r="C86" s="9" t="s">
+      <c r="C86" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D86" s="14" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E86" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
+        <v>795</v>
+      </c>
+      <c r="B87" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="B87" s="23"/>
-      <c r="C87" s="9" t="s">
+      <c r="C87" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D87" s="14" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E87" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
+        <v>796</v>
+      </c>
+      <c r="B88" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="B88" s="23"/>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D88" s="14" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E88" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
+        <v>797</v>
+      </c>
+      <c r="B89" s="10" t="s">
         <v>497</v>
       </c>
-      <c r="B89" s="23"/>
-      <c r="C89" s="9" t="s">
+      <c r="C89" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D89" s="14" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E89" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
+        <v>798</v>
+      </c>
+      <c r="B90" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="B90" s="23"/>
-      <c r="C90" s="9" t="s">
+      <c r="C90" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D90" s="14" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E90" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="B91" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="B91" s="23"/>
-      <c r="C91" s="9" t="s">
+      <c r="C91" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D91" s="14" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E91" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
+        <v>800</v>
+      </c>
+      <c r="B92" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="B92" s="23"/>
-      <c r="C92" s="9" t="s">
+      <c r="C92" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D92" s="14" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E92" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="B93" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="B93" s="23"/>
-      <c r="C93" s="9" t="s">
+      <c r="C93" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D93" s="14" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E93" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
+        <v>802</v>
+      </c>
+      <c r="B94" s="10" t="s">
         <v>499</v>
       </c>
-      <c r="B94" s="23"/>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D94" s="14" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E94" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
+        <v>803</v>
+      </c>
+      <c r="B95" s="10" t="s">
         <v>500</v>
       </c>
-      <c r="B95" s="23"/>
-      <c r="C95" s="9" t="s">
+      <c r="C95" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D95" s="14" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E95" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
+        <v>804</v>
+      </c>
+      <c r="B96" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="B96" s="23"/>
-      <c r="C96" s="9" t="s">
+      <c r="C96" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D96" s="14" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E96" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
+        <v>805</v>
+      </c>
+      <c r="B97" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="B97" s="23"/>
-      <c r="C97" s="9" t="s">
+      <c r="C97" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D97" s="14" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E97" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
+        <v>806</v>
+      </c>
+      <c r="B98" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="B98" s="23"/>
-      <c r="C98" s="9" t="s">
+      <c r="C98" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D98" s="14" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E98" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F98" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
+        <v>807</v>
+      </c>
+      <c r="B99" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="B99" s="23"/>
-      <c r="C99" s="9" t="s">
+      <c r="C99" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D99" s="14" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E99" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F99" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
+        <v>808</v>
+      </c>
+      <c r="B100" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="B100" s="23"/>
-      <c r="C100" s="9" t="s">
+      <c r="C100" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D100" s="14" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E100" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F100" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="B101" s="10" t="s">
         <v>501</v>
       </c>
-      <c r="B101" s="23"/>
-      <c r="C101" s="9" t="s">
+      <c r="C101" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D101" s="14" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E101" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
+        <v>810</v>
+      </c>
+      <c r="B102" s="10" t="s">
         <v>502</v>
       </c>
-      <c r="B102" s="23"/>
-      <c r="C102" s="9" t="s">
+      <c r="C102" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D102" s="14" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E102" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F102" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="B103" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="B103" s="23"/>
-      <c r="C103" s="9" t="s">
+      <c r="C103" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D103" s="14" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E103" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F103" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="B104" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="B104" s="23"/>
-      <c r="C104" s="9" t="s">
+      <c r="C104" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D104" s="14" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E104" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F104" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="B105" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="B105" s="23"/>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D105" s="14" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E105" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F105" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
+        <v>814</v>
+      </c>
+      <c r="B106" s="10" t="s">
         <v>506</v>
       </c>
-      <c r="B106" s="23"/>
-      <c r="C106" s="9" t="s">
+      <c r="C106" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D106" s="14" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E106" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F106" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
+        <v>815</v>
+      </c>
+      <c r="B107" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="B107" s="23"/>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D107" s="14" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E107" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F107" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
+        <v>816</v>
+      </c>
+      <c r="B108" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="B108" s="23"/>
-      <c r="C108" s="9" t="s">
+      <c r="C108" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D108" s="14" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E108" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F108" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="B109" s="10" t="s">
         <v>508</v>
       </c>
-      <c r="B109" s="23"/>
-      <c r="C109" s="9" t="s">
+      <c r="C109" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D109" s="14" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E109" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F109" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
+        <v>818</v>
+      </c>
+      <c r="B110" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="B110" s="23"/>
-      <c r="C110" s="9" t="s">
+      <c r="C110" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D110" s="14" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E110" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F110" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
+        <v>819</v>
+      </c>
+      <c r="B111" s="10" t="s">
         <v>510</v>
       </c>
-      <c r="B111" s="23"/>
-      <c r="C111" s="9" t="s">
+      <c r="C111" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D111" s="14" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E111" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F111" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="B112" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B112" s="23"/>
-      <c r="C112" s="9" t="s">
+      <c r="C112" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D112" s="14" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E112" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F112" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
+        <v>821</v>
+      </c>
+      <c r="B113" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="B113" s="23"/>
-      <c r="C113" s="9" t="s">
+      <c r="C113" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D113" s="14" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E113" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F113" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
+        <v>822</v>
+      </c>
+      <c r="B114" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="B114" s="23"/>
-      <c r="C114" s="9" t="s">
+      <c r="C114" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D114" s="14" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E114" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F114" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
+        <v>823</v>
+      </c>
+      <c r="B115" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="B115" s="23"/>
-      <c r="C115" s="9" t="s">
+      <c r="C115" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D115" s="14" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E115" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F115" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
+        <v>824</v>
+      </c>
+      <c r="B116" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="B116" s="23"/>
-      <c r="C116" s="9" t="s">
+      <c r="C116" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D116" s="14" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E116" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F116" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
+        <v>825</v>
+      </c>
+      <c r="B117" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="B117" s="23"/>
-      <c r="C117" s="9" t="s">
+      <c r="C117" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D117" s="14" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E117" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F117" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
+        <v>826</v>
+      </c>
+      <c r="B118" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="B118" s="23"/>
-      <c r="C118" s="9" t="s">
+      <c r="C118" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D118" s="14" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E118" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F118" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
+        <v>827</v>
+      </c>
+      <c r="B119" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="B119" s="23"/>
-      <c r="C119" s="9" t="s">
+      <c r="C119" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D119" s="14" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E119" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F119" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="B120" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="B120" s="23"/>
-      <c r="C120" s="9" t="s">
+      <c r="C120" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D120" s="14" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E120" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F120" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="B121" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="B121" s="23"/>
-      <c r="C121" s="9" t="s">
+      <c r="C121" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D121" s="14" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E121" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F121" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
+        <v>830</v>
+      </c>
+      <c r="B122" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="B122" s="23"/>
-      <c r="C122" s="9" t="s">
+      <c r="C122" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D122" s="14" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E122" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F122" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="B123" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="B123" s="23"/>
-      <c r="C123" s="9" t="s">
+      <c r="C123" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D123" s="14" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E123" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F123" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="B124" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="B124" s="23"/>
-      <c r="C124" s="9" t="s">
+      <c r="C124" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D124" s="14" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E124" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F124" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="B125" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="B125" s="23"/>
-      <c r="C125" s="9" t="s">
+      <c r="C125" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D125" s="14" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E125" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F125" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="B126" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="B126" s="23"/>
-      <c r="C126" s="9" t="s">
+      <c r="C126" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D126" s="14" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E126" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F126" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
+        <v>835</v>
+      </c>
+      <c r="B127" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="B127" s="23"/>
-      <c r="C127" s="9" t="s">
+      <c r="C127" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D127" s="14" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E127" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F127" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="B128" s="10" t="s">
         <v>460</v>
       </c>
-      <c r="B128" s="23"/>
-      <c r="C128" s="9" t="s">
+      <c r="C128" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D128" s="14" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E128" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F128" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="B129" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="B129" s="23"/>
-      <c r="C129" s="9" t="s">
+      <c r="C129" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D129" s="14" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E129" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F129" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="B130" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="B130" s="23"/>
-      <c r="C130" s="9" t="s">
+      <c r="C130" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D130" s="14" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E130" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F130" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="B131" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="B131" s="23"/>
-      <c r="C131" s="9" t="s">
+      <c r="C131" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D131" s="14" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E131" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F131" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="B132" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="B132" s="23"/>
-      <c r="C132" s="9" t="s">
+      <c r="C132" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="D132" s="14" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="10" t="s">
+      <c r="E132" s="36" t="s">
+        <v>841</v>
+      </c>
+      <c r="F132" s="14" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B133" s="10" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="10" t="s">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B134" s="10" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="10" t="s">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B135" s="10" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="10" t="s">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B136" s="10" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="10" t="s">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B137" s="10" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="10" t="s">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B138" s="10" t="s">
         <v>513</v>
       </c>
     </row>
@@ -6056,6 +7957,91 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD128"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" style="3" customWidth="1"/>
+    <col min="2" max="2" width="125.33203125" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>844</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>846</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="23"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="23"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="23"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -6486,34 +8472,34 @@
       <c r="A3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -6633,16 +8619,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes and updated readme
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/amendment_1.xlsx
+++ b/tests/integration_test_files/amendment_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD347573-AC53-554C-ABBC-B12CFE0D6C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BBFE10-C785-5A4D-969F-5C34C7D6FE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20100" yWindow="500" windowWidth="53160" windowHeight="27240" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="20100" yWindow="500" windowWidth="53160" windowHeight="27240" activeTab="15" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="852">
   <si>
     <t>Screening</t>
   </si>
@@ -2633,12 +2633,21 @@
   <si>
     <t>document</t>
   </si>
+  <si>
+    <t>intercurrentEventText</t>
+  </si>
+  <si>
+    <t>ICE Text</t>
+  </si>
+  <si>
+    <t>populationSubset</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2664,14 +2673,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2721,7 +2722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2748,10 +2749,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2794,17 +2791,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2819,6 +2807,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3146,12 +3143,12 @@
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="6" width="24.6640625" style="25" customWidth="1"/>
+    <col min="5" max="6" width="24.6640625" style="23" customWidth="1"/>
     <col min="7" max="7" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>446</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -3159,7 +3156,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -3167,15 +3164,15 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -3183,7 +3180,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -3191,7 +3188,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -3199,7 +3196,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -3207,15 +3204,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>110</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -3223,7 +3220,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="16" t="s">
         <v>111</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -3231,7 +3228,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>112</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -3239,7 +3236,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="16" t="s">
         <v>113</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -3247,15 +3244,15 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>115</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -3263,25 +3260,25 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="16" t="s">
         <v>518</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>519</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="16" t="s">
         <v>531</v>
       </c>
     </row>
@@ -3301,7 +3298,7 @@
       <c r="E17" t="s">
         <v>528</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="24">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
@@ -3324,7 +3321,7 @@
       <c r="E18" t="s">
         <v>529</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
@@ -3347,7 +3344,7 @@
       <c r="E19" t="s">
         <v>529</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="24">
         <v>44958</v>
       </c>
       <c r="G19" t="s">
@@ -3370,7 +3367,7 @@
       <c r="E20" t="s">
         <v>529</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="24">
         <v>44988</v>
       </c>
       <c r="G20" t="s">
@@ -3393,7 +3390,7 @@
       <c r="E21" t="s">
         <v>529</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="24">
         <v>44988</v>
       </c>
       <c r="G21" t="s">
@@ -3416,7 +3413,7 @@
       <c r="E22" t="s">
         <v>529</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="24">
         <v>44988</v>
       </c>
       <c r="G22" t="s">
@@ -3439,7 +3436,7 @@
       <c r="E23" t="s">
         <v>529</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="24">
         <v>44988</v>
       </c>
       <c r="G23" t="s">
@@ -3655,16 +3652,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3732,61 +3729,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>446</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>564</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>565</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>566</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>567</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>568</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="19" t="s">
         <v>569</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="19" t="s">
         <v>570</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="19" t="s">
         <v>571</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="19" t="s">
         <v>573</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="19" t="s">
         <v>574</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="19" t="s">
         <v>575</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="19" t="s">
         <v>576</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="19" t="s">
         <v>577</v>
       </c>
     </row>
@@ -3806,7 +3803,7 @@
       <c r="E2" t="s">
         <v>651</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>581</v>
       </c>
       <c r="G2" t="s">
@@ -3845,7 +3842,7 @@
       <c r="R2" t="s">
         <v>591</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="S2" s="27" t="s">
         <v>592</v>
       </c>
     </row>
@@ -3865,7 +3862,7 @@
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="26" t="s">
         <v>581</v>
       </c>
       <c r="G3" t="s">
@@ -3904,7 +3901,7 @@
       <c r="R3" t="s">
         <v>591</v>
       </c>
-      <c r="S3" s="29" t="s">
+      <c r="S3" s="27" t="s">
         <v>592</v>
       </c>
     </row>
@@ -3929,16 +3926,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>446</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3980,7 +3977,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3995,28 +3992,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>599</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>446</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>519</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>600</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>601</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>607</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="17" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4087,37 +4084,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>553</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>554</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>555</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>556</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>557</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="19" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4633,49 +4630,56 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="61.83203125" customWidth="1"/>
+    <col min="3" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" customWidth="1"/>
+    <col min="7" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="61.83203125" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="19" t="s">
+        <v>851</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J1" s="19" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -4686,32 +4690,44 @@
         <v>100</v>
       </c>
       <c r="D2" t="s">
+        <v>605</v>
+      </c>
+      <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>105</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>76</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>83</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3" t="s">
+      <c r="J2" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H4" t="s">
+      <c r="J3" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -4722,19 +4738,25 @@
         <v>100</v>
       </c>
       <c r="D5" t="s">
+        <v>606</v>
+      </c>
+      <c r="E5" t="s">
         <v>134</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>135</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>84</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>136</v>
+      </c>
+      <c r="J5" t="s">
+        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -4765,22 +4787,22 @@
       <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4853,28 +4875,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>166</v>
       </c>
     </row>
@@ -5010,19 +5032,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>166</v>
       </c>
     </row>
@@ -5121,13 +5143,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051C019D-8DBE-D14B-A9B5-0060B58D7557}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" style="25" customWidth="1"/>
+    <col min="1" max="1" width="11" style="23" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="5" width="25.5" customWidth="1"/>
@@ -5136,28 +5158,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>532</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>533</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>534</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>535</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>656</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>544</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>520</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>848</v>
       </c>
     </row>
@@ -5189,7 +5211,7 @@
       <c r="A3" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>536</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -5275,28 +5297,28 @@
     <col min="1" max="1" width="9.33203125" style="10" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" style="10" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46" style="14" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="46" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="32" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="30" t="s">
         <v>446</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="30" t="s">
         <v>486</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="28" t="s">
         <v>707</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="28" t="s">
         <v>708</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="29" t="s">
         <v>709</v>
       </c>
     </row>
@@ -5307,16 +5329,16 @@
       <c r="B2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>842</v>
       </c>
     </row>
@@ -5327,16 +5349,16 @@
       <c r="B3" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="C3" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5347,16 +5369,16 @@
       <c r="B4" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5367,16 +5389,16 @@
       <c r="B5" s="10" t="s">
         <v>383</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E5" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5387,16 +5409,16 @@
       <c r="B6" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="C6" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="E6" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5407,16 +5429,16 @@
       <c r="B7" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5427,16 +5449,16 @@
       <c r="B8" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="E8" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5447,16 +5469,16 @@
       <c r="B9" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="E9" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F9" s="14" t="s">
+      <c r="E9" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5464,19 +5486,19 @@
       <c r="A10" s="10" t="s">
         <v>718</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>515</v>
       </c>
-      <c r="E10" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>843</v>
       </c>
     </row>
@@ -5487,16 +5509,16 @@
       <c r="B11" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="E11" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F11" s="14" t="s">
+      <c r="E11" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5507,16 +5529,16 @@
       <c r="B12" s="10" t="s">
         <v>389</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="E12" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F12" s="14" t="s">
+      <c r="E12" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5527,16 +5549,16 @@
       <c r="B13" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="C13" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="C13" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="E13" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="E13" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5547,16 +5569,16 @@
       <c r="B14" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="E14" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F14" s="14" t="s">
+      <c r="E14" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5567,16 +5589,16 @@
       <c r="B15" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="E15" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F15" s="14" t="s">
+      <c r="E15" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5587,16 +5609,16 @@
       <c r="B16" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D16" s="14" t="s">
+      <c r="C16" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="E16" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F16" s="14" t="s">
+      <c r="E16" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5607,16 +5629,16 @@
       <c r="B17" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="C17" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="E17" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F17" s="14" t="s">
+      <c r="E17" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5627,16 +5649,16 @@
       <c r="B18" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="C18" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D18" s="14" t="s">
+      <c r="C18" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="E18" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F18" s="14" t="s">
+      <c r="E18" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5647,16 +5669,16 @@
       <c r="B19" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="C19" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D19" s="14" t="s">
+      <c r="C19" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="E19" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F19" s="14" t="s">
+      <c r="E19" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5667,16 +5689,16 @@
       <c r="B20" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="C20" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="E20" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5687,16 +5709,16 @@
       <c r="B21" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="C21" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D21" s="14" t="s">
+      <c r="C21" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="E21" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F21" s="14" t="s">
+      <c r="E21" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5707,16 +5729,16 @@
       <c r="B22" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="C22" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D22" s="14" t="s">
+      <c r="C22" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="E22" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F22" s="14" t="s">
+      <c r="E22" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5727,16 +5749,16 @@
       <c r="B23" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="C23" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D23" s="14" t="s">
+      <c r="C23" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="E23" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F23" s="14" t="s">
+      <c r="E23" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>844</v>
       </c>
     </row>
@@ -5747,16 +5769,16 @@
       <c r="B24" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="C24" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D24" s="14" t="s">
+      <c r="C24" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="E24" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F24" s="14" t="s">
+      <c r="E24" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>845</v>
       </c>
     </row>
@@ -5767,16 +5789,16 @@
       <c r="B25" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="C25" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="C25" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="E25" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F25" s="14" t="s">
+      <c r="E25" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5787,16 +5809,16 @@
       <c r="B26" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="C26" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D26" s="14" t="s">
+      <c r="C26" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="E26" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F26" s="14" t="s">
+      <c r="E26" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5807,16 +5829,16 @@
       <c r="B27" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="C27" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D27" s="14" t="s">
+      <c r="C27" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="E27" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F27" s="14" t="s">
+      <c r="E27" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5827,16 +5849,16 @@
       <c r="B28" s="10" t="s">
         <v>438</v>
       </c>
-      <c r="C28" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D28" s="14" t="s">
+      <c r="C28" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="E28" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5847,16 +5869,16 @@
       <c r="B29" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="C29" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D29" s="14" t="s">
+      <c r="C29" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="E29" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F29" s="14" t="s">
+      <c r="E29" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5867,16 +5889,16 @@
       <c r="B30" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="C30" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D30" s="14" t="s">
+      <c r="C30" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="E30" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F30" s="14" t="s">
+      <c r="E30" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5887,16 +5909,16 @@
       <c r="B31" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="C31" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D31" s="14" t="s">
+      <c r="C31" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="E31" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F31" s="14" t="s">
+      <c r="E31" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5907,16 +5929,16 @@
       <c r="B32" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="C32" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D32" s="14" t="s">
+      <c r="C32" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="E32" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F32" s="14" t="s">
+      <c r="E32" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5927,16 +5949,16 @@
       <c r="B33" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="C33" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D33" s="14" t="s">
+      <c r="C33" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="E33" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F33" s="14" t="s">
+      <c r="E33" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5947,16 +5969,16 @@
       <c r="B34" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="C34" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D34" s="14" t="s">
+      <c r="C34" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="E34" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F34" s="14" t="s">
+      <c r="E34" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F34" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5967,16 +5989,16 @@
       <c r="B35" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="C35" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D35" s="14" t="s">
+      <c r="C35" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D35" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="E35" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F35" s="14" t="s">
+      <c r="E35" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F35" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -5987,16 +6009,16 @@
       <c r="B36" s="10" t="s">
         <v>480</v>
       </c>
-      <c r="C36" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D36" s="14" t="s">
+      <c r="C36" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="E36" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F36" s="14" t="s">
+      <c r="E36" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6007,16 +6029,16 @@
       <c r="B37" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="C37" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D37" s="14" t="s">
+      <c r="C37" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="E37" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F37" s="14" t="s">
+      <c r="E37" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6027,16 +6049,16 @@
       <c r="B38" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="C38" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D38" s="14" t="s">
+      <c r="C38" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D38" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="E38" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F38" s="14" t="s">
+      <c r="E38" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F38" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6047,16 +6069,16 @@
       <c r="B39" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="C39" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D39" s="14" t="s">
+      <c r="C39" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="E39" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F39" s="14" t="s">
+      <c r="E39" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F39" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6067,16 +6089,16 @@
       <c r="B40" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="C40" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D40" s="14" t="s">
+      <c r="C40" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D40" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="E40" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F40" s="14" t="s">
+      <c r="E40" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F40" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6087,16 +6109,16 @@
       <c r="B41" s="10" t="s">
         <v>482</v>
       </c>
-      <c r="C41" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D41" s="14" t="s">
+      <c r="C41" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="E41" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F41" s="14" t="s">
+      <c r="E41" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F41" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6107,16 +6129,16 @@
       <c r="B42" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="C42" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D42" s="14" t="s">
+      <c r="C42" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D42" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="E42" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F42" s="14" t="s">
+      <c r="E42" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F42" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6127,16 +6149,16 @@
       <c r="B43" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="C43" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D43" s="14" t="s">
+      <c r="C43" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D43" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="E43" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F43" s="14" t="s">
+      <c r="E43" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F43" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6147,16 +6169,16 @@
       <c r="B44" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="C44" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D44" s="14" t="s">
+      <c r="C44" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="E44" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F44" s="14" t="s">
+      <c r="E44" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F44" s="12" t="s">
         <v>846</v>
       </c>
     </row>
@@ -6167,16 +6189,16 @@
       <c r="B45" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C45" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D45" s="14" t="s">
+      <c r="C45" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D45" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="E45" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F45" s="14" t="s">
+      <c r="E45" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F45" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6187,16 +6209,16 @@
       <c r="B46" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="C46" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D46" s="14" t="s">
+      <c r="C46" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D46" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E46" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F46" s="14" t="s">
+      <c r="E46" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F46" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6207,16 +6229,16 @@
       <c r="B47" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="C47" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D47" s="14" t="s">
+      <c r="C47" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="E47" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F47" s="14" t="s">
+      <c r="E47" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6227,16 +6249,16 @@
       <c r="B48" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="C48" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D48" s="14" t="s">
+      <c r="C48" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="E48" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F48" s="14" t="s">
+      <c r="E48" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F48" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6247,16 +6269,16 @@
       <c r="B49" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="C49" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D49" s="14" t="s">
+      <c r="C49" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="E49" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F49" s="14" t="s">
+      <c r="E49" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F49" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6267,16 +6289,16 @@
       <c r="B50" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="C50" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D50" s="14" t="s">
+      <c r="C50" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="E50" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F50" s="14" t="s">
+      <c r="E50" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F50" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6287,16 +6309,16 @@
       <c r="B51" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="C51" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D51" s="14" t="s">
+      <c r="C51" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="E51" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F51" s="14" t="s">
+      <c r="E51" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F51" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6307,16 +6329,16 @@
       <c r="B52" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="C52" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D52" s="14" t="s">
+      <c r="C52" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="E52" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F52" s="14" t="s">
+      <c r="E52" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F52" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6327,16 +6349,16 @@
       <c r="B53" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="C53" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D53" s="14" t="s">
+      <c r="C53" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="E53" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F53" s="14" t="s">
+      <c r="E53" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F53" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6347,16 +6369,16 @@
       <c r="B54" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="C54" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D54" s="14" t="s">
+      <c r="C54" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D54" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="E54" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F54" s="14" t="s">
+      <c r="E54" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F54" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6367,16 +6389,16 @@
       <c r="B55" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="C55" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D55" s="14" t="s">
+      <c r="C55" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D55" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="E55" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F55" s="14" t="s">
+      <c r="E55" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F55" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6387,16 +6409,16 @@
       <c r="B56" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="C56" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D56" s="14" t="s">
+      <c r="C56" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="E56" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F56" s="14" t="s">
+      <c r="E56" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F56" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6407,16 +6429,16 @@
       <c r="B57" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="C57" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D57" s="14" t="s">
+      <c r="C57" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="E57" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F57" s="14" t="s">
+      <c r="E57" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F57" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6427,16 +6449,16 @@
       <c r="B58" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="C58" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D58" s="14" t="s">
+      <c r="C58" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D58" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="E58" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F58" s="14" t="s">
+      <c r="E58" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F58" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6447,16 +6469,16 @@
       <c r="B59" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="C59" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D59" s="14" t="s">
+      <c r="C59" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D59" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="E59" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F59" s="14" t="s">
+      <c r="E59" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F59" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6467,16 +6489,16 @@
       <c r="B60" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="C60" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D60" s="14" t="s">
+      <c r="C60" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D60" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="E60" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F60" s="14" t="s">
+      <c r="E60" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F60" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6487,16 +6509,16 @@
       <c r="B61" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="C61" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D61" s="14" t="s">
+      <c r="C61" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D61" s="12" t="s">
         <v>307</v>
       </c>
-      <c r="E61" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F61" s="14" t="s">
+      <c r="E61" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F61" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6507,16 +6529,16 @@
       <c r="B62" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="C62" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D62" s="14" t="s">
+      <c r="C62" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D62" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="E62" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F62" s="14" t="s">
+      <c r="E62" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F62" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6527,16 +6549,16 @@
       <c r="B63" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="C63" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D63" s="14" t="s">
+      <c r="C63" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>309</v>
       </c>
-      <c r="E63" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F63" s="14" t="s">
+      <c r="E63" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F63" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6547,16 +6569,16 @@
       <c r="B64" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="C64" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D64" s="14" t="s">
+      <c r="C64" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D64" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="E64" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F64" s="14" t="s">
+      <c r="E64" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F64" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6567,16 +6589,16 @@
       <c r="B65" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="C65" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D65" s="14" t="s">
+      <c r="C65" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>311</v>
       </c>
-      <c r="E65" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F65" s="14" t="s">
+      <c r="E65" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F65" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6587,16 +6609,16 @@
       <c r="B66" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="C66" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D66" s="14" t="s">
+      <c r="C66" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="E66" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F66" s="14" t="s">
+      <c r="E66" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6607,16 +6629,16 @@
       <c r="B67" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="C67" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D67" s="14" t="s">
+      <c r="C67" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="E67" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F67" s="14" t="s">
+      <c r="E67" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F67" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6627,16 +6649,16 @@
       <c r="B68" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="C68" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D68" s="14" t="s">
+      <c r="C68" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D68" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="E68" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F68" s="14" t="s">
+      <c r="E68" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F68" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6647,16 +6669,16 @@
       <c r="B69" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="C69" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D69" s="14" t="s">
+      <c r="C69" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D69" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="E69" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F69" s="14" t="s">
+      <c r="E69" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F69" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6667,16 +6689,16 @@
       <c r="B70" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="C70" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D70" s="14" t="s">
+      <c r="C70" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D70" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="E70" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F70" s="14" t="s">
+      <c r="E70" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F70" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6687,16 +6709,16 @@
       <c r="B71" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="C71" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D71" s="14" t="s">
+      <c r="C71" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D71" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="E71" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F71" s="14" t="s">
+      <c r="E71" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F71" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6707,16 +6729,16 @@
       <c r="B72" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="C72" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D72" s="14" t="s">
+      <c r="C72" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D72" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="E72" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F72" s="14" t="s">
+      <c r="E72" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F72" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6727,16 +6749,16 @@
       <c r="B73" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="C73" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D73" s="14" t="s">
+      <c r="C73" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D73" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="E73" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F73" s="14" t="s">
+      <c r="E73" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F73" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6747,16 +6769,16 @@
       <c r="B74" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="C74" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D74" s="14" t="s">
+      <c r="C74" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D74" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="E74" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F74" s="14" t="s">
+      <c r="E74" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F74" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6767,16 +6789,16 @@
       <c r="B75" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="C75" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D75" s="14" t="s">
+      <c r="C75" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D75" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="E75" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F75" s="14" t="s">
+      <c r="E75" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F75" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6787,16 +6809,16 @@
       <c r="B76" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="C76" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D76" s="14" t="s">
+      <c r="C76" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D76" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="E76" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F76" s="14" t="s">
+      <c r="E76" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F76" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6807,16 +6829,16 @@
       <c r="B77" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="C77" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D77" s="14" t="s">
+      <c r="C77" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D77" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="E77" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F77" s="14" t="s">
+      <c r="E77" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F77" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6827,16 +6849,16 @@
       <c r="B78" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="C78" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D78" s="14" t="s">
+      <c r="C78" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D78" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="E78" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F78" s="14" t="s">
+      <c r="E78" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F78" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6847,16 +6869,16 @@
       <c r="B79" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="C79" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D79" s="14" t="s">
+      <c r="C79" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D79" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="E79" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F79" s="14" t="s">
+      <c r="E79" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F79" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6867,16 +6889,16 @@
       <c r="B80" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="C80" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D80" s="14" t="s">
+      <c r="C80" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D80" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="E80" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F80" s="14" t="s">
+      <c r="E80" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F80" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6887,16 +6909,16 @@
       <c r="B81" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="C81" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D81" s="14" t="s">
+      <c r="C81" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D81" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="E81" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F81" s="14" t="s">
+      <c r="E81" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F81" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6907,16 +6929,16 @@
       <c r="B82" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="C82" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D82" s="14" t="s">
+      <c r="C82" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D82" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="E82" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F82" s="14" t="s">
+      <c r="E82" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F82" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6927,16 +6949,16 @@
       <c r="B83" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="C83" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D83" s="14" t="s">
+      <c r="C83" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D83" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="E83" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F83" s="14" t="s">
+      <c r="E83" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F83" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6947,16 +6969,16 @@
       <c r="B84" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="C84" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D84" s="14" t="s">
+      <c r="C84" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D84" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="E84" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F84" s="14" t="s">
+      <c r="E84" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F84" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6967,16 +6989,16 @@
       <c r="B85" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="C85" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D85" s="14" t="s">
+      <c r="C85" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D85" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="E85" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F85" s="14" t="s">
+      <c r="E85" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F85" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -6987,16 +7009,16 @@
       <c r="B86" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="C86" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D86" s="14" t="s">
+      <c r="C86" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D86" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="E86" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F86" s="14" t="s">
+      <c r="E86" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F86" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7007,16 +7029,16 @@
       <c r="B87" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="C87" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D87" s="14" t="s">
+      <c r="C87" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D87" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="E87" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F87" s="14" t="s">
+      <c r="E87" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F87" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7027,16 +7049,16 @@
       <c r="B88" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="C88" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D88" s="14" t="s">
+      <c r="C88" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D88" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="E88" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F88" s="14" t="s">
+      <c r="E88" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F88" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7047,16 +7069,16 @@
       <c r="B89" s="10" t="s">
         <v>497</v>
       </c>
-      <c r="C89" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D89" s="14" t="s">
+      <c r="C89" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D89" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="E89" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F89" s="14" t="s">
+      <c r="E89" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F89" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7067,16 +7089,16 @@
       <c r="B90" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="C90" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D90" s="14" t="s">
+      <c r="C90" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D90" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="E90" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F90" s="14" t="s">
+      <c r="E90" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F90" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7087,16 +7109,16 @@
       <c r="B91" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="C91" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D91" s="14" t="s">
+      <c r="C91" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D91" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="E91" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F91" s="14" t="s">
+      <c r="E91" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F91" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7107,16 +7129,16 @@
       <c r="B92" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="C92" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D92" s="14" t="s">
+      <c r="C92" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D92" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="E92" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F92" s="14" t="s">
+      <c r="E92" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F92" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7127,16 +7149,16 @@
       <c r="B93" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="C93" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D93" s="14" t="s">
+      <c r="C93" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D93" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="E93" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F93" s="14" t="s">
+      <c r="E93" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F93" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7147,16 +7169,16 @@
       <c r="B94" s="10" t="s">
         <v>499</v>
       </c>
-      <c r="C94" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D94" s="14" t="s">
+      <c r="C94" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D94" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="E94" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F94" s="14" t="s">
+      <c r="E94" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F94" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7167,16 +7189,16 @@
       <c r="B95" s="10" t="s">
         <v>500</v>
       </c>
-      <c r="C95" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D95" s="14" t="s">
+      <c r="C95" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D95" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="E95" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F95" s="14" t="s">
+      <c r="E95" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F95" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7187,16 +7209,16 @@
       <c r="B96" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="C96" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D96" s="14" t="s">
+      <c r="C96" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D96" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E96" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F96" s="14" t="s">
+      <c r="E96" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F96" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7207,16 +7229,16 @@
       <c r="B97" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="C97" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D97" s="14" t="s">
+      <c r="C97" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D97" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="E97" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F97" s="14" t="s">
+      <c r="E97" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F97" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7227,16 +7249,16 @@
       <c r="B98" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="C98" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D98" s="14" t="s">
+      <c r="C98" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D98" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="E98" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F98" s="14" t="s">
+      <c r="E98" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F98" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7247,16 +7269,16 @@
       <c r="B99" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="C99" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D99" s="14" t="s">
+      <c r="C99" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D99" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E99" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F99" s="14" t="s">
+      <c r="E99" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F99" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7267,16 +7289,16 @@
       <c r="B100" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="C100" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D100" s="14" t="s">
+      <c r="C100" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D100" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="E100" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F100" s="14" t="s">
+      <c r="E100" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F100" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7287,16 +7309,16 @@
       <c r="B101" s="10" t="s">
         <v>501</v>
       </c>
-      <c r="C101" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D101" s="14" t="s">
+      <c r="C101" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D101" s="12" t="s">
         <v>347</v>
       </c>
-      <c r="E101" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F101" s="14" t="s">
+      <c r="E101" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F101" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7307,16 +7329,16 @@
       <c r="B102" s="10" t="s">
         <v>502</v>
       </c>
-      <c r="C102" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D102" s="14" t="s">
+      <c r="C102" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D102" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="E102" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F102" s="14" t="s">
+      <c r="E102" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F102" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7327,16 +7349,16 @@
       <c r="B103" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="C103" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D103" s="14" t="s">
+      <c r="C103" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D103" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="E103" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F103" s="14" t="s">
+      <c r="E103" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F103" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7347,16 +7369,16 @@
       <c r="B104" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="C104" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D104" s="14" t="s">
+      <c r="C104" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D104" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="E104" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F104" s="14" t="s">
+      <c r="E104" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F104" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7367,16 +7389,16 @@
       <c r="B105" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="C105" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D105" s="14" t="s">
+      <c r="C105" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D105" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="E105" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F105" s="14" t="s">
+      <c r="E105" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F105" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7387,16 +7409,16 @@
       <c r="B106" s="10" t="s">
         <v>506</v>
       </c>
-      <c r="C106" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D106" s="14" t="s">
+      <c r="C106" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D106" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="E106" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F106" s="14" t="s">
+      <c r="E106" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F106" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7407,16 +7429,16 @@
       <c r="B107" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="C107" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D107" s="14" t="s">
+      <c r="C107" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D107" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="E107" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F107" s="14" t="s">
+      <c r="E107" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F107" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7427,16 +7449,16 @@
       <c r="B108" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="C108" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D108" s="14" t="s">
+      <c r="C108" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D108" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="E108" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F108" s="14" t="s">
+      <c r="E108" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F108" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7447,16 +7469,16 @@
       <c r="B109" s="10" t="s">
         <v>508</v>
       </c>
-      <c r="C109" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D109" s="14" t="s">
+      <c r="C109" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D109" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="E109" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F109" s="14" t="s">
+      <c r="E109" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F109" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7467,16 +7489,16 @@
       <c r="B110" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="C110" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D110" s="14" t="s">
+      <c r="C110" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D110" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="E110" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F110" s="14" t="s">
+      <c r="E110" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F110" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7487,16 +7509,16 @@
       <c r="B111" s="10" t="s">
         <v>510</v>
       </c>
-      <c r="C111" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D111" s="14" t="s">
+      <c r="C111" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D111" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="E111" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F111" s="14" t="s">
+      <c r="E111" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F111" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7507,16 +7529,16 @@
       <c r="B112" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="C112" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D112" s="14" t="s">
+      <c r="C112" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D112" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="E112" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F112" s="14" t="s">
+      <c r="E112" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F112" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7527,16 +7549,16 @@
       <c r="B113" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="C113" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D113" s="14" t="s">
+      <c r="C113" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D113" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="E113" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F113" s="14" t="s">
+      <c r="E113" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F113" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7547,16 +7569,16 @@
       <c r="B114" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="C114" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D114" s="14" t="s">
+      <c r="C114" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D114" s="12" t="s">
         <v>360</v>
       </c>
-      <c r="E114" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F114" s="14" t="s">
+      <c r="E114" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F114" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7567,16 +7589,16 @@
       <c r="B115" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="C115" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D115" s="14" t="s">
+      <c r="C115" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D115" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="E115" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F115" s="14" t="s">
+      <c r="E115" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F115" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7587,16 +7609,16 @@
       <c r="B116" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="C116" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D116" s="14" t="s">
+      <c r="C116" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D116" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="E116" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F116" s="14" t="s">
+      <c r="E116" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F116" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7607,16 +7629,16 @@
       <c r="B117" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="C117" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D117" s="14" t="s">
+      <c r="C117" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D117" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="E117" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F117" s="14" t="s">
+      <c r="E117" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F117" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7627,16 +7649,16 @@
       <c r="B118" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="C118" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D118" s="14" t="s">
+      <c r="C118" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D118" s="12" t="s">
         <v>364</v>
       </c>
-      <c r="E118" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F118" s="14" t="s">
+      <c r="E118" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F118" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7647,16 +7669,16 @@
       <c r="B119" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="C119" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D119" s="14" t="s">
+      <c r="C119" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D119" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="E119" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F119" s="14" t="s">
+      <c r="E119" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F119" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7667,16 +7689,16 @@
       <c r="B120" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="C120" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D120" s="14" t="s">
+      <c r="C120" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D120" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="E120" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F120" s="14" t="s">
+      <c r="E120" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F120" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7687,16 +7709,16 @@
       <c r="B121" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="C121" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D121" s="14" t="s">
+      <c r="C121" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D121" s="12" t="s">
         <v>367</v>
       </c>
-      <c r="E121" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F121" s="14" t="s">
+      <c r="E121" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F121" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7707,16 +7729,16 @@
       <c r="B122" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C122" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D122" s="14" t="s">
+      <c r="C122" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D122" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="E122" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F122" s="14" t="s">
+      <c r="E122" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F122" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7727,16 +7749,16 @@
       <c r="B123" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="C123" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D123" s="14" t="s">
+      <c r="C123" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D123" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="E123" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F123" s="14" t="s">
+      <c r="E123" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F123" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7747,16 +7769,16 @@
       <c r="B124" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="C124" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D124" s="14" t="s">
+      <c r="C124" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D124" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="E124" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F124" s="14" t="s">
+      <c r="E124" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F124" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7767,16 +7789,16 @@
       <c r="B125" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="C125" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D125" s="14" t="s">
+      <c r="C125" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D125" s="12" t="s">
         <v>371</v>
       </c>
-      <c r="E125" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F125" s="14" t="s">
+      <c r="E125" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F125" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7787,16 +7809,16 @@
       <c r="B126" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="C126" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D126" s="14" t="s">
+      <c r="C126" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D126" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="E126" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F126" s="14" t="s">
+      <c r="E126" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F126" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7807,16 +7829,16 @@
       <c r="B127" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="C127" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D127" s="14" t="s">
+      <c r="C127" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D127" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="E127" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F127" s="14" t="s">
+      <c r="E127" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F127" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7827,16 +7849,16 @@
       <c r="B128" s="10" t="s">
         <v>460</v>
       </c>
-      <c r="C128" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D128" s="14" t="s">
+      <c r="C128" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D128" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="E128" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F128" s="14" t="s">
+      <c r="E128" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F128" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7847,16 +7869,16 @@
       <c r="B129" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="C129" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D129" s="14" t="s">
+      <c r="C129" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D129" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="E129" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F129" s="14" t="s">
+      <c r="E129" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F129" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7867,16 +7889,16 @@
       <c r="B130" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="C130" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D130" s="14" t="s">
+      <c r="C130" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D130" s="12" t="s">
         <v>376</v>
       </c>
-      <c r="E130" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F130" s="14" t="s">
+      <c r="E130" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F130" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7887,16 +7909,16 @@
       <c r="B131" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="C131" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D131" s="14" t="s">
+      <c r="C131" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D131" s="12" t="s">
         <v>377</v>
       </c>
-      <c r="E131" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F131" s="14" t="s">
+      <c r="E131" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F131" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7907,16 +7929,16 @@
       <c r="B132" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="C132" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="D132" s="14" t="s">
+      <c r="C132" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="D132" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="E132" s="36" t="s">
-        <v>841</v>
-      </c>
-      <c r="F132" s="14" t="s">
+      <c r="E132" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="F132" s="12" t="s">
         <v>847</v>
       </c>
     </row>
@@ -7971,15 +7993,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>446</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>842</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -7995,7 +8017,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>844</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -8011,7 +8033,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>846</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -8019,21 +8041,21 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="21" t="s">
         <v>847</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
+      <c r="A8" s="21"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
+      <c r="A9" s="21"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
+      <c r="A10" s="21"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
+      <c r="A11" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -8094,25 +8116,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>519</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>660</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>533</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>672</v>
       </c>
     </row>
@@ -8240,23 +8262,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="25" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="23" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>661</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>46</v>
       </c>
     </row>
@@ -8367,22 +8389,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -8447,115 +8469,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>185</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -8619,16 +8641,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8652,19 +8674,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>235</v>
       </c>
     </row>
@@ -8726,13 +8748,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>222</v>
       </c>
     </row>
@@ -8806,13 +8828,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>142</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>446</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -8832,13 +8854,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -8858,13 +8880,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>146</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>519</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -8884,8 +8906,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="13"/>
+      <c r="C4" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -8905,8 +8927,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="C5" s="15" t="s">
+      <c r="A5" s="13"/>
+      <c r="C5" s="13" t="s">
         <v>620</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -8926,8 +8948,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="C6" s="15" t="s">
+      <c r="A6" s="13"/>
+      <c r="C6" s="13" t="s">
         <v>622</v>
       </c>
       <c r="D6" s="2"/>
@@ -8939,7 +8961,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>623</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -8961,7 +8983,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>624</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -8981,13 +9003,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Amendment name, label and description chnage, DDF-RA #625
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/amendment_1.xlsx
+++ b/tests/integration_test_files/amendment_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88065AB-D14F-8844-A7FD-F1056132B478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40084D1B-9FCD-C24B-BF75-15672F4C1595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51580" yWindow="500" windowWidth="51200" windowHeight="27240" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="27240" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="862">
   <si>
     <t>Screening</t>
   </si>
@@ -2645,6 +2645,33 @@
   </si>
   <si>
     <t>spare</t>
+  </si>
+  <si>
+    <t>AMEND_1</t>
+  </si>
+  <si>
+    <t>AMEND_2</t>
+  </si>
+  <si>
+    <t>AMEND_3</t>
+  </si>
+  <si>
+    <t>AMEND_4</t>
+  </si>
+  <si>
+    <t>Amendment 4</t>
+  </si>
+  <si>
+    <t>Amendment One</t>
+  </si>
+  <si>
+    <t>Amendment Two</t>
+  </si>
+  <si>
+    <t>Amendment Three</t>
+  </si>
+  <si>
+    <t>Amendment Four</t>
   </si>
 </sst>
 </file>
@@ -5275,145 +5302,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051C019D-8DBE-D14B-A9B5-0060B58D7557}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" style="23" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="5" width="25.5" customWidth="1"/>
-    <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11" style="23" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="7" max="8" width="25.5" customWidth="1"/>
+    <col min="9" max="9" width="34" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>440</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>526</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>527</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>528</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>529</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>650</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>538</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>514</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>853</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>661</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>858</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>531</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
         <v>518</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>541</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>695</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>854</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>660</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>859</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>530</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
         <v>651</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>542</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>698</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>855</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>659</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>535</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>536</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>537</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>856</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>857</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>861</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>539</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>540</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
         <v>652</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>700</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>842</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8759,7 +8834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>